<commit_message>
feat: KYC & KYC intergation (WIP)
</commit_message>
<xml_diff>
--- a/src/app/modules/kyc/kyc_models/MVP-2-KYC-Commons-22_dev.xlsx
+++ b/src/app/modules/kyc/kyc_models/MVP-2-KYC-Commons-22_dev.xlsx
@@ -205,13 +205,13 @@
     <t xml:space="preserve">Prénom</t>
   </si>
   <si>
-    <t xml:space="preserve">prenom</t>
+    <t xml:space="preserve">first_name</t>
   </si>
   <si>
     <t xml:space="preserve">Nom</t>
   </si>
   <si>
-    <t xml:space="preserve">nom</t>
+    <t xml:space="preserve">last_name</t>
   </si>
   <si>
     <t xml:space="preserve">Pseudo</t>
@@ -818,7 +818,7 @@
     <t xml:space="preserve">Hobbies &amp; Convivialité</t>
   </si>
   <si>
-    <t xml:space="preserve">Hobbies</t>
+    <t xml:space="preserve">Intérêts / hobbies</t>
   </si>
   <si>
     <t xml:space="preserve">hobbies</t>
@@ -1686,10 +1686,12 @@
   </sheetPr>
   <dimension ref="A1:AML1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="6410" ySplit="0" topLeftCell="D51" activePane="bottomLeft" state="split"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="10741" ySplit="2627" topLeftCell="G41" activePane="bottomLeft" state="split"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topRight" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
+      <selection pane="bottomRight" activeCell="G41" activeCellId="0" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4609375" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2705,8 +2707,8 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
       <c r="M20" s="4"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>

</xml_diff>